<commit_message>
antes de corrigir os erros da tabela BrightStarMultiple
</commit_message>
<xml_diff>
--- a/Biostar_Catalogue/output_files/CAT1/csv/CAT1_estrelas_sem_G_e_estrelas_sem_Bp_Rp.xlsx
+++ b/Biostar_Catalogue/output_files/CAT1/csv/CAT1_estrelas_sem_G_e_estrelas_sem_Bp_Rp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="sem_G" sheetId="1" state="visible" r:id="rId3"/>
@@ -435,8 +435,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -634,155 +638,156 @@
   </sheetPr>
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="10.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="5.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="4.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="5.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="5.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>16.909328</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <v>16.4556684056988</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>0.00587043480049942</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>16.678308</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <v>16.8570752272611</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>0.00396938381021705</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>10.086929</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>8.826408</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>9.0706433182189</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="I5" s="1" t="n">
         <v>0.00501990443946543</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="1" t="n">
         <v>7.8101223182189</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="1" t="n">
         <v>0.00501990443946498</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="L5" s="1" t="n">
         <v>1.260521</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>16.847324</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="1" t="n">
         <v>17.5516661551832</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>0.0033672801484137</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>18.6281</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="1" t="n">
         <v>17.6475947077668</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>0.0248717994857604</v>
       </c>
     </row>
@@ -804,1392 +809,1392 @@
   </sheetPr>
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>13.639243</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>13.342862776382</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>0.0033251291503662</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>12.822794</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>11.5075603982448</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>0.00296077718730281</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>12.650045</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>11.1991539791241</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>0.00278745963019134</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>11.717453</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>11.3754344010533</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>0.00166568898743336</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>15.768858</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>15.5725597485765</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>0.0021575360997117</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>12.654424</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>11.2291884887719</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>0.00234350675565764</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>20.418549</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>19.1098736768072</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>0.129551767896416</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>20.71029</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>19.6701101476339</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>0.0977739443121628</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>20.568031</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>19.415993315235</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>0.0730825349447439</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>15.510378</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>14.0386075500702</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>0.00432028191084566</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>20.698986</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>20.1094781964312</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>0.0792371528832057</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>20.831068</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>19.482100644615</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>0.114883425222317</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>20.793224</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>18.9236524342615</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>0.145609937331523</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>20.301674</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>19.0061338057685</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>0.0378608834495164</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>11.64075</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>11.0213709675566</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>0.00154372819332238</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>11.583294</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>10.1298732690345</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>0.00203589886982591</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>14.60586</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>13.1176024354998</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>0.0044002750528076</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>12.3821945</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>10.9118787191696</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>0.00496846431059872</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>10.395799</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <v>9.55173550863484</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="1" t="n">
         <v>0.00564373995172129</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>11.697051</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <v>10.8021862837445</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="1" t="n">
         <v>0.005587111094707</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>20.577303</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>20.42117</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="1" t="n">
         <v>20.4470185291875</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="1" t="n">
         <v>0.024845353626116</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="1" t="n">
         <v>20.2908855291875</v>
       </c>
-      <c r="I22" s="0" t="n">
+      <c r="I22" s="1" t="n">
         <v>0.024845353626116</v>
       </c>
-      <c r="N22" s="0" t="n">
+      <c r="N22" s="1" t="n">
         <v>-0.156133</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>10.839606</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="1" t="n">
         <v>9.61181157926333</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23" s="1" t="n">
         <v>0.00619478906124549</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>13.93621</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="1" t="n">
         <v>12.4452953399592</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="1" t="n">
         <v>0.00352674033546219</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>12.853741</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="1" t="n">
         <v>12.0770699952645</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <v>0.0129678773779443</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>11.070571</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>8.683837</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="1" t="n">
         <v>9.59794893378707</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="1" t="n">
         <v>0.00244796974173678</v>
       </c>
-      <c r="J26" s="0" t="n">
+      <c r="J26" s="1" t="n">
         <v>7.21121493378707</v>
       </c>
-      <c r="K26" s="0" t="n">
+      <c r="K26" s="1" t="n">
         <v>0.00244796974173678</v>
       </c>
-      <c r="M26" s="0" t="n">
+      <c r="M26" s="1" t="n">
         <v>2.386734</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>20.037308</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="1" t="n">
         <v>19.6002690002286</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="1" t="n">
         <v>0.0769132598215006</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>19.925434</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="1" t="n">
         <v>18.4909835197785</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="G28" s="1" t="n">
         <v>0.105949944346094</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>19.689613</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29" s="1" t="n">
         <v>18.1352503729856</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="G29" s="1" t="n">
         <v>0.0655411408247755</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>19.791285</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="1" t="n">
         <v>18.2627291503373</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="1" t="n">
         <v>0.0969775491455938</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="1" t="n">
         <v>19.840805</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31" s="1" t="n">
         <v>18.2545987445285</v>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="G31" s="1" t="n">
         <v>0.0580179917492085</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="C32" s="1" t="n">
         <v>20.299034</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32" s="1" t="n">
         <v>18.3920392201958</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="G32" s="1" t="n">
         <v>0.163622755656851</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="C33" s="1" t="n">
         <v>20.016611</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33" s="1" t="n">
         <v>18.3011640824823</v>
       </c>
-      <c r="G33" s="0" t="n">
+      <c r="G33" s="1" t="n">
         <v>0.0930338718872328</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C34" s="1" t="n">
         <v>19.556583</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F34" s="1" t="n">
         <v>18.4275242858687</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G34" s="1" t="n">
         <v>0.0437739024500718</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C35" s="1" t="n">
         <v>19.57727</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F35" s="1" t="n">
         <v>17.9994397921536</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="G35" s="1" t="n">
         <v>0.0905190501880195</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36" s="1" t="n">
         <v>19.215883</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F36" s="1" t="n">
         <v>17.6220619830601</v>
       </c>
-      <c r="G36" s="0" t="n">
+      <c r="G36" s="1" t="n">
         <v>0.0816357665524041</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37" s="1" t="n">
         <v>19.787502</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F37" s="1" t="n">
         <v>18.7815718121982</v>
       </c>
-      <c r="G37" s="0" t="n">
+      <c r="G37" s="1" t="n">
         <v>0.0568377236174928</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39" s="1" t="n">
         <v>20.339483</v>
       </c>
-      <c r="F39" s="0" t="n">
+      <c r="F39" s="1" t="n">
         <v>18.9215280650603</v>
       </c>
-      <c r="G39" s="0" t="n">
+      <c r="G39" s="1" t="n">
         <v>0.101187533531265</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="C40" s="1" t="n">
         <v>19.727787</v>
       </c>
-      <c r="F40" s="0" t="n">
+      <c r="F40" s="1" t="n">
         <v>18.3269112328658</v>
       </c>
-      <c r="G40" s="0" t="n">
+      <c r="G40" s="1" t="n">
         <v>0.0730025432725991</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C41" s="1" t="n">
         <v>20.250418</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="F41" s="1" t="n">
         <v>18.4854501756083</v>
       </c>
-      <c r="G41" s="0" t="n">
+      <c r="G41" s="1" t="n">
         <v>0.102678239482346</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42" s="1" t="n">
         <v>19.863749</v>
       </c>
-      <c r="F42" s="0" t="n">
+      <c r="F42" s="1" t="n">
         <v>18.3758690116394</v>
       </c>
-      <c r="G42" s="0" t="n">
+      <c r="G42" s="1" t="n">
         <v>0.112805400612224</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="C43" s="1" t="n">
         <v>20.34856</v>
       </c>
-      <c r="F43" s="0" t="n">
+      <c r="F43" s="1" t="n">
         <v>19.044691082934</v>
       </c>
-      <c r="G43" s="0" t="n">
+      <c r="G43" s="1" t="n">
         <v>0.0954876283513428</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="C44" s="1" t="n">
         <v>19.984222</v>
       </c>
-      <c r="F44" s="0" t="n">
+      <c r="F44" s="1" t="n">
         <v>18.4619661185026</v>
       </c>
-      <c r="G44" s="0" t="n">
+      <c r="G44" s="1" t="n">
         <v>0.0929602643022047</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C45" s="0" t="n">
+      <c r="C45" s="1" t="n">
         <v>20.066053</v>
       </c>
-      <c r="F45" s="0" t="n">
+      <c r="F45" s="1" t="n">
         <v>18.3767712833423</v>
       </c>
-      <c r="G45" s="0" t="n">
+      <c r="G45" s="1" t="n">
         <v>0.100282071580368</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C46" s="0" t="n">
+      <c r="C46" s="1" t="n">
         <v>20.371605</v>
       </c>
-      <c r="F46" s="0" t="n">
+      <c r="F46" s="1" t="n">
         <v>18.6757712465346</v>
       </c>
-      <c r="G46" s="0" t="n">
+      <c r="G46" s="1" t="n">
         <v>0.127972640099891</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="0" t="n">
+      <c r="C47" s="1" t="n">
         <v>20.452175</v>
       </c>
-      <c r="F47" s="0" t="n">
+      <c r="F47" s="1" t="n">
         <v>18.7546647865308</v>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="G47" s="1" t="n">
         <v>0.131727055880241</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C48" s="0" t="n">
+      <c r="C48" s="1" t="n">
         <v>20.471943</v>
       </c>
-      <c r="F48" s="0" t="n">
+      <c r="F48" s="1" t="n">
         <v>18.7860782196909</v>
       </c>
-      <c r="G48" s="0" t="n">
+      <c r="G48" s="1" t="n">
         <v>0.147646283633696</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C49" s="0" t="n">
+      <c r="C49" s="1" t="n">
         <v>20.670315</v>
       </c>
-      <c r="F49" s="0" t="n">
+      <c r="F49" s="1" t="n">
         <v>19.1669167355974</v>
       </c>
-      <c r="G49" s="0" t="n">
+      <c r="G49" s="1" t="n">
         <v>0.129880328613192</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="0" t="n">
+      <c r="E50" s="1" t="n">
         <v>16.909328</v>
       </c>
-      <c r="J50" s="0" t="n">
+      <c r="J50" s="1" t="n">
         <v>16.4556684056988</v>
       </c>
-      <c r="K50" s="0" t="n">
+      <c r="K50" s="1" t="n">
         <v>0.00587043480049942</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C51" s="0" t="n">
+      <c r="C51" s="1" t="n">
         <v>20.53789</v>
       </c>
-      <c r="F51" s="0" t="n">
+      <c r="F51" s="1" t="n">
         <v>18.6884162552983</v>
       </c>
-      <c r="G51" s="0" t="n">
+      <c r="G51" s="1" t="n">
         <v>0.125924076192511</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C52" s="0" t="n">
+      <c r="C52" s="1" t="n">
         <v>20.525904</v>
       </c>
-      <c r="F52" s="0" t="n">
+      <c r="F52" s="1" t="n">
         <v>18.6710629361123</v>
       </c>
-      <c r="G52" s="0" t="n">
+      <c r="G52" s="1" t="n">
         <v>0.151089934930827</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C53" s="0" t="n">
+      <c r="C53" s="1" t="n">
         <v>19.755878</v>
       </c>
-      <c r="F53" s="0" t="n">
+      <c r="F53" s="1" t="n">
         <v>18.0558571764711</v>
       </c>
-      <c r="G53" s="0" t="n">
+      <c r="G53" s="1" t="n">
         <v>0.0874571165573421</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C54" s="0" t="n">
+      <c r="C54" s="1" t="n">
         <v>20.276348</v>
       </c>
-      <c r="F54" s="0" t="n">
+      <c r="F54" s="1" t="n">
         <v>18.6058261901541</v>
       </c>
-      <c r="G54" s="0" t="n">
+      <c r="G54" s="1" t="n">
         <v>0.14314129059289</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C55" s="0" t="n">
+      <c r="C55" s="1" t="n">
         <v>20.119987</v>
       </c>
-      <c r="F55" s="0" t="n">
+      <c r="F55" s="1" t="n">
         <v>19.1391605383039</v>
       </c>
-      <c r="G55" s="0" t="n">
+      <c r="G55" s="1" t="n">
         <v>0.0842127547264742</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C56" s="0" t="n">
+      <c r="C56" s="1" t="n">
         <v>20.3671</v>
       </c>
-      <c r="F56" s="0" t="n">
+      <c r="F56" s="1" t="n">
         <v>18.7120938593635</v>
       </c>
-      <c r="G56" s="0" t="n">
+      <c r="G56" s="1" t="n">
         <v>0.109867546895167</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C57" s="0" t="n">
+      <c r="C57" s="1" t="n">
         <v>20.040459</v>
       </c>
-      <c r="F57" s="0" t="n">
+      <c r="F57" s="1" t="n">
         <v>18.5110071232838</v>
       </c>
-      <c r="G57" s="0" t="n">
+      <c r="G57" s="1" t="n">
         <v>0.0723761653803479</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="0" t="n">
+      <c r="C58" s="1" t="n">
         <v>20.029032</v>
       </c>
-      <c r="F58" s="0" t="n">
+      <c r="F58" s="1" t="n">
         <v>19.6604255396683</v>
       </c>
-      <c r="G58" s="0" t="n">
+      <c r="G58" s="1" t="n">
         <v>0.0639791837785246</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C59" s="0" t="n">
+      <c r="C59" s="1" t="n">
         <v>12.295122</v>
       </c>
-      <c r="F59" s="0" t="n">
+      <c r="F59" s="1" t="n">
         <v>11.0444954504399</v>
       </c>
-      <c r="G59" s="0" t="n">
+      <c r="G59" s="1" t="n">
         <v>0.00189590815386787</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="0" t="n">
+      <c r="C60" s="1" t="n">
         <v>19.897444</v>
       </c>
-      <c r="E60" s="0" t="n">
+      <c r="E60" s="1" t="n">
         <v>18.201824</v>
       </c>
-      <c r="F60" s="0" t="n">
+      <c r="F60" s="1" t="n">
         <v>18.5945081701632</v>
       </c>
-      <c r="G60" s="0" t="n">
+      <c r="G60" s="1" t="n">
         <v>0.0228080723599788</v>
       </c>
-      <c r="J60" s="0" t="n">
+      <c r="J60" s="1" t="n">
         <v>16.8988881701632</v>
       </c>
-      <c r="K60" s="0" t="n">
+      <c r="K60" s="1" t="n">
         <v>0.0228080723599806</v>
       </c>
-      <c r="M60" s="0" t="n">
+      <c r="M60" s="1" t="n">
         <v>1.69562</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C61" s="0" t="n">
+      <c r="C61" s="1" t="n">
         <v>12.988087</v>
       </c>
-      <c r="F61" s="0" t="n">
+      <c r="F61" s="1" t="n">
         <v>12.0597603291822</v>
       </c>
-      <c r="G61" s="0" t="n">
+      <c r="G61" s="1" t="n">
         <v>0.00427943666759045</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C62" s="0" t="n">
+      <c r="C62" s="1" t="n">
         <v>19.90784</v>
       </c>
-      <c r="F62" s="0" t="n">
+      <c r="F62" s="1" t="n">
         <v>18.387978755396</v>
       </c>
-      <c r="G62" s="0" t="n">
+      <c r="G62" s="1" t="n">
         <v>0.106641856075134</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C63" s="0" t="n">
+      <c r="C63" s="1" t="n">
         <v>20.46364</v>
       </c>
-      <c r="F63" s="0" t="n">
+      <c r="F63" s="1" t="n">
         <v>18.6021610305838</v>
       </c>
-      <c r="G63" s="0" t="n">
+      <c r="G63" s="1" t="n">
         <v>0.171626508881705</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C64" s="0" t="n">
+      <c r="C64" s="1" t="n">
         <v>20.093605</v>
       </c>
-      <c r="F64" s="0" t="n">
+      <c r="F64" s="1" t="n">
         <v>18.3117669350706</v>
       </c>
-      <c r="G64" s="0" t="n">
+      <c r="G64" s="1" t="n">
         <v>0.113473857718441</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C65" s="0" t="n">
+      <c r="C65" s="1" t="n">
         <v>20.840277</v>
       </c>
-      <c r="F65" s="0" t="n">
+      <c r="F65" s="1" t="n">
         <v>19.8054797154462</v>
       </c>
-      <c r="G65" s="0" t="n">
+      <c r="G65" s="1" t="n">
         <v>0.136499939560522</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C66" s="0" t="n">
+      <c r="C66" s="1" t="n">
         <v>20.618402</v>
       </c>
-      <c r="F66" s="0" t="n">
+      <c r="F66" s="1" t="n">
         <v>20.6417644504754</v>
       </c>
-      <c r="G66" s="0" t="n">
+      <c r="G66" s="1" t="n">
         <v>0.0745345006042317</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E67" s="0" t="n">
+      <c r="E67" s="1" t="n">
         <v>16.678308</v>
       </c>
-      <c r="J67" s="0" t="n">
+      <c r="J67" s="1" t="n">
         <v>16.8570752272611</v>
       </c>
-      <c r="K67" s="0" t="n">
+      <c r="K67" s="1" t="n">
         <v>0.00396938381021705</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C68" s="0" t="n">
+      <c r="C68" s="1" t="n">
         <v>20.518063</v>
       </c>
-      <c r="F68" s="0" t="n">
+      <c r="F68" s="1" t="n">
         <v>18.6678670143873</v>
       </c>
-      <c r="G68" s="0" t="n">
+      <c r="G68" s="1" t="n">
         <v>0.188044531464307</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="0" t="n">
+      <c r="C69" s="1" t="n">
         <v>12.034219</v>
       </c>
-      <c r="F69" s="0" t="n">
+      <c r="F69" s="1" t="n">
         <v>11.3621930576386</v>
       </c>
-      <c r="G69" s="0" t="n">
+      <c r="G69" s="1" t="n">
         <v>0.00266073875420503</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C70" s="0" t="n">
+      <c r="C70" s="1" t="n">
         <v>12.5353</v>
       </c>
-      <c r="F70" s="0" t="n">
+      <c r="F70" s="1" t="n">
         <v>11.0712152021881</v>
       </c>
-      <c r="G70" s="0" t="n">
+      <c r="G70" s="1" t="n">
         <v>0.00847487877074826</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C71" s="0" t="n">
+      <c r="C71" s="1" t="n">
         <v>13.531994</v>
       </c>
-      <c r="F71" s="0" t="n">
+      <c r="F71" s="1" t="n">
         <v>12.6737810614086</v>
       </c>
-      <c r="G71" s="0" t="n">
+      <c r="G71" s="1" t="n">
         <v>0.00225593907924626</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C72" s="0" t="n">
+      <c r="C72" s="1" t="n">
         <v>16.191395</v>
       </c>
-      <c r="F72" s="0" t="n">
+      <c r="F72" s="1" t="n">
         <v>14.9113673527172</v>
       </c>
-      <c r="G72" s="0" t="n">
+      <c r="G72" s="1" t="n">
         <v>0.00448223786932456</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C73" s="0" t="n">
+      <c r="C73" s="1" t="n">
         <v>13.0888405</v>
       </c>
-      <c r="F73" s="0" t="n">
+      <c r="F73" s="1" t="n">
         <v>12.9222719223097</v>
       </c>
-      <c r="G73" s="0" t="n">
+      <c r="G73" s="1" t="n">
         <v>0.00369062588412206</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C74" s="0" t="n">
+      <c r="C74" s="1" t="n">
         <v>14.638643</v>
       </c>
-      <c r="F74" s="0" t="n">
+      <c r="F74" s="1" t="n">
         <v>13.3241348462558</v>
       </c>
-      <c r="G74" s="0" t="n">
+      <c r="G74" s="1" t="n">
         <v>0.00349811228558483</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C75" s="0" t="n">
+      <c r="C75" s="1" t="n">
         <v>13.44563</v>
       </c>
-      <c r="F75" s="0" t="n">
+      <c r="F75" s="1" t="n">
         <v>13.7032979134062</v>
       </c>
-      <c r="G75" s="0" t="n">
+      <c r="G75" s="1" t="n">
         <v>0.00252349407356167</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C76" s="0" t="n">
+      <c r="C76" s="1" t="n">
         <v>12.365336</v>
       </c>
-      <c r="F76" s="0" t="n">
+      <c r="F76" s="1" t="n">
         <v>12.3185086810707</v>
       </c>
-      <c r="G76" s="0" t="n">
+      <c r="G76" s="1" t="n">
         <v>0.00199197710215948</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C77" s="0" t="n">
+      <c r="C77" s="1" t="n">
         <v>11.1696205</v>
       </c>
-      <c r="F77" s="0" t="n">
+      <c r="F77" s="1" t="n">
         <v>10.2849921552474</v>
       </c>
-      <c r="G77" s="0" t="n">
+      <c r="G77" s="1" t="n">
         <v>0.000814082115567771</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E78" s="0" t="n">
+      <c r="E78" s="1" t="n">
         <v>16.847324</v>
       </c>
-      <c r="J78" s="0" t="n">
+      <c r="J78" s="1" t="n">
         <v>17.5516661551832</v>
       </c>
-      <c r="K78" s="0" t="n">
+      <c r="K78" s="1" t="n">
         <v>0.0033672801484137</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C79" s="0" t="n">
+      <c r="C79" s="1" t="n">
         <v>20.948887</v>
       </c>
-      <c r="F79" s="0" t="n">
+      <c r="F79" s="1" t="n">
         <v>19.0938163127813</v>
       </c>
-      <c r="G79" s="0" t="n">
+      <c r="G79" s="1" t="n">
         <v>0.171664166705803</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C80" s="0" t="n">
+      <c r="C80" s="1" t="n">
         <v>20.707253</v>
       </c>
-      <c r="F80" s="0" t="n">
+      <c r="F80" s="1" t="n">
         <v>18.7493704908856</v>
       </c>
-      <c r="G80" s="0" t="n">
+      <c r="G80" s="1" t="n">
         <v>0.184886365204452</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C81" s="0" t="n">
+      <c r="C81" s="1" t="n">
         <v>19.542095</v>
       </c>
-      <c r="F81" s="0" t="n">
+      <c r="F81" s="1" t="n">
         <v>17.8595329851473</v>
       </c>
-      <c r="G81" s="0" t="n">
+      <c r="G81" s="1" t="n">
         <v>0.0914849113390464</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C82" s="0" t="n">
+      <c r="C82" s="1" t="n">
         <v>12.00015</v>
       </c>
-      <c r="F82" s="0" t="n">
+      <c r="F82" s="1" t="n">
         <v>11.0525314777659</v>
       </c>
-      <c r="G82" s="0" t="n">
+      <c r="G82" s="1" t="n">
         <v>0.00304132251564049</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C83" s="0" t="n">
+      <c r="C83" s="1" t="n">
         <v>19.838758</v>
       </c>
-      <c r="F83" s="0" t="n">
+      <c r="F83" s="1" t="n">
         <v>18.5083650510155</v>
       </c>
-      <c r="G83" s="0" t="n">
+      <c r="G83" s="1" t="n">
         <v>0.0210086525563398</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C84" s="0" t="n">
+      <c r="C84" s="1" t="n">
         <v>20.291456</v>
       </c>
-      <c r="F84" s="0" t="n">
+      <c r="F84" s="1" t="n">
         <v>18.676081296248</v>
       </c>
-      <c r="G84" s="0" t="n">
+      <c r="G84" s="1" t="n">
         <v>0.0951205932741939</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C85" s="0" t="n">
+      <c r="C85" s="1" t="n">
         <v>20.491726</v>
       </c>
-      <c r="F85" s="0" t="n">
+      <c r="F85" s="1" t="n">
         <v>18.8508340706256</v>
       </c>
-      <c r="G85" s="0" t="n">
+      <c r="G85" s="1" t="n">
         <v>0.140683604552059</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="A86" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B86" s="0" t="s">
+      <c r="B86" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C86" s="0" t="n">
+      <c r="C86" s="1" t="n">
         <v>11.334182</v>
       </c>
-      <c r="F86" s="0" t="n">
+      <c r="F86" s="1" t="n">
         <v>10.1958249161587</v>
       </c>
-      <c r="G86" s="0" t="n">
+      <c r="G86" s="1" t="n">
         <v>0.00403275825928695</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+      <c r="A87" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C87" s="0" t="n">
+      <c r="C87" s="1" t="n">
         <v>12.732754</v>
       </c>
-      <c r="F87" s="0" t="n">
+      <c r="F87" s="1" t="n">
         <v>12.3979601719456</v>
       </c>
-      <c r="G87" s="0" t="n">
+      <c r="G87" s="1" t="n">
         <v>0.00288499511998008</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+      <c r="A88" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E88" s="0" t="n">
+      <c r="E88" s="1" t="n">
         <v>18.6281</v>
       </c>
-      <c r="J88" s="0" t="n">
+      <c r="J88" s="1" t="n">
         <v>17.6475947077668</v>
       </c>
-      <c r="K88" s="0" t="n">
+      <c r="K88" s="1" t="n">
         <v>0.0248717994857604</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="A89" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C89" s="0" t="n">
+      <c r="C89" s="1" t="n">
         <v>12.93071</v>
       </c>
-      <c r="E89" s="0" t="n">
+      <c r="E89" s="1" t="n">
         <v>10.643531</v>
       </c>
-      <c r="F89" s="0" t="n">
+      <c r="F89" s="1" t="n">
         <v>11.8462799329652</v>
       </c>
-      <c r="G89" s="0" t="n">
+      <c r="G89" s="1" t="n">
         <v>0.00521560973569635</v>
       </c>
-      <c r="J89" s="0" t="n">
+      <c r="J89" s="1" t="n">
         <v>9.55910093296517</v>
       </c>
-      <c r="K89" s="0" t="n">
+      <c r="K89" s="1" t="n">
         <v>0.00521560973569635</v>
       </c>
-      <c r="M89" s="0" t="n">
+      <c r="M89" s="1" t="n">
         <v>2.287179</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+      <c r="A90" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C90" s="0" t="n">
+      <c r="C90" s="1" t="n">
         <v>12.269101</v>
       </c>
-      <c r="F90" s="0" t="n">
+      <c r="F90" s="1" t="n">
         <v>11.8780891189774</v>
       </c>
-      <c r="G90" s="0" t="n">
+      <c r="G90" s="1" t="n">
         <v>0.00340879940289707</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+      <c r="A91" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C91" s="0" t="n">
+      <c r="C91" s="1" t="n">
         <v>12.560951</v>
       </c>
-      <c r="F91" s="0" t="n">
+      <c r="F91" s="1" t="n">
         <v>11.1784213875247</v>
       </c>
-      <c r="G91" s="0" t="n">
+      <c r="G91" s="1" t="n">
         <v>0.00237363662364132</v>
       </c>
     </row>

</xml_diff>

<commit_message>
antes de mudar o input do Gaia para a forma programática
</commit_message>
<xml_diff>
--- a/Biostar_Catalogue/output_files/CAT1/csv/CAT1_estrelas_sem_G_e_estrelas_sem_Bp_Rp.xlsx
+++ b/Biostar_Catalogue/output_files/CAT1/csv/CAT1_estrelas_sem_G_e_estrelas_sem_Bp_Rp.xlsx
@@ -638,8 +638,8 @@
   </sheetPr>
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -651,8 +651,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="4.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.6"/>

</xml_diff>